<commit_message>
Smk imod python conversion #1 (NBr32)
README.md + how_to_make_Env.md update
Mdl_Prep -> unfinshed
</commit_message>
<xml_diff>
--- a/Mng/Mdl_Ipvs.xlsx
+++ b/Mng/Mdl_Ipvs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD745F49-56FE-4B0D-9D3E-06D8F7B6DACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E7195C-042B-4DF1-BDEA-ACB69337B244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,7 +673,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294964216" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="329">
   <si>
     <t>#</t>
   </si>

</xml_diff>